<commit_message>
0109 SQL 과제 제출
0109 SQL 과제 제출입니다.
</commit_message>
<xml_diff>
--- a/0109 SQL/24기 김종진 sql 과제 2.xlsx
+++ b/0109 SQL/24기 김종진 sql 과제 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a372ece13d04507e/바탕 화면/와이빅타/과제/0109 SQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17B78519-8A75-4227-9754-71DB778B0FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{17B78519-8A75-4227-9754-71DB778B0FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC72D804-E853-4A88-BE71-72BAF16D67C2}"/>
   <bookViews>
     <workbookView xWindow="8670" yWindow="2520" windowWidth="18630" windowHeight="12840" xr2:uid="{FBC60233-994D-4D53-AAC6-D192002A284A}"/>
   </bookViews>
@@ -210,7 +210,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,13 +249,6 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -307,7 +300,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -320,16 +313,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -646,30 +633,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02445966-8E81-4FD0-A7E3-FAB98C3591F6}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.375" customWidth="1"/>
     <col min="2" max="4" width="21" customWidth="1"/>
     <col min="7" max="8" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
@@ -680,7 +667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -690,7 +677,6 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4"/>
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
@@ -701,7 +687,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -711,7 +697,6 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4"/>
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
@@ -722,7 +707,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -732,7 +717,6 @@
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4"/>
       <c r="E4" s="1" t="s">
         <v>36</v>
       </c>
@@ -743,7 +727,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -753,7 +737,6 @@
       <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4"/>
       <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
@@ -764,7 +747,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -774,7 +757,6 @@
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4"/>
       <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
@@ -785,7 +767,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -795,7 +777,6 @@
       <c r="C7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="4"/>
       <c r="E7" s="1" t="s">
         <v>33</v>
       </c>
@@ -806,7 +787,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -816,7 +797,6 @@
       <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="4"/>
       <c r="E8" s="1" t="s">
         <v>35</v>
       </c>
@@ -827,7 +807,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -837,9 +817,8 @@
       <c r="C9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:7">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -849,7 +828,6 @@
       <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="4"/>
       <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
@@ -857,7 +835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -867,7 +845,6 @@
       <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="4"/>
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
@@ -875,7 +852,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -885,7 +862,6 @@
       <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="4"/>
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
@@ -893,7 +869,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -903,7 +879,6 @@
       <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="4"/>
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
@@ -911,7 +886,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -921,7 +896,6 @@
       <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="4"/>
       <c r="E14" s="1" t="s">
         <v>31</v>
       </c>
@@ -929,7 +903,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -939,7 +913,6 @@
       <c r="C15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="4"/>
       <c r="E15" s="1" t="s">
         <v>32</v>
       </c>
@@ -947,7 +920,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -957,7 +930,6 @@
       <c r="C16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="4"/>
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
@@ -965,15 +937,11 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
       <c r="E18" s="2" t="s">
         <v>0</v>
       </c>
@@ -984,11 +952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
@@ -999,11 +963,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1014,11 +974,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E21" s="1" t="s">
         <v>37</v>
       </c>
@@ -1029,11 +985,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E22" s="1" t="s">
         <v>39</v>
       </c>
@@ -1044,11 +996,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E23" s="1" t="s">
         <v>40</v>
       </c>
@@ -1059,11 +1007,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E24" s="1" t="s">
         <v>41</v>
       </c>
@@ -1073,65 +1017,6 @@
       <c r="G24" s="1">
         <v>1970</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>